<commit_message>
Implement Week 1: Modern CSS architecture and Theo mode
- Restructure CSS into modular system (variables, reset, typography, layout, components, animations)
- Add Theo mode dark theme with toggle button and localStorage persistence
- Integrate Inter font from Google Fonts with fluid typography
- Add pillar column support to build.py (PREDICT, PREVENT, PERSONALIZE)
- Update DataForSite.xlsx with pillar column for projects
- Implement pillar validation in build pipeline

Co-Authored-By: Claude Sonnet 4.5 <noreply@anthropic.com>
</commit_message>
<xml_diff>
--- a/DataForSite.xlsx
+++ b/DataForSite.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/diego/Coding Things/vs code projects/northwellsite/futuristic northwell site /"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B7B97C9F-4F96-6644-800E-1773D940569D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5D66370E-09D9-DF46-B4A4-9B7C42324583}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="660" windowWidth="30240" windowHeight="18980" activeTab="2" xr2:uid="{3A380ED6-0686-C94C-8463-1D265E34B0D0}"/>
+    <workbookView xWindow="0" yWindow="660" windowWidth="30240" windowHeight="18980" activeTab="1" xr2:uid="{3A380ED6-0686-C94C-8463-1D265E34B0D0}"/>
   </bookViews>
   <sheets>
     <sheet name="Researchers" sheetId="1" r:id="rId1"/>
@@ -80,7 +80,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="44">
   <si>
     <t xml:space="preserve">Researcher Name </t>
   </si>
@@ -203,6 +203,15 @@
   </si>
   <si>
     <t>https://github.com/delton4/DivisionofHealthAI</t>
+  </si>
+  <si>
+    <t>Project Pillar</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Predict </t>
+  </si>
+  <si>
+    <t>Personalize</t>
   </si>
 </sst>
 </file>
@@ -680,7 +689,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B4C4F324-8489-E645-BB21-4ACA0F14EF43}">
   <dimension ref="A1:G3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="D1" zoomScale="244" workbookViewId="0">
       <selection activeCell="C29" sqref="C29"/>
     </sheetView>
   </sheetViews>
@@ -768,10 +777,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{73191352-1248-7143-B4CD-49A6A0426C0D}">
-  <dimension ref="A1:G3"/>
+  <dimension ref="A1:H3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B29" sqref="B29"/>
+    <sheetView tabSelected="1" zoomScale="112" workbookViewId="0">
+      <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -785,7 +794,7 @@
     <col min="7" max="7" width="23" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>19</v>
       </c>
@@ -807,8 +816,11 @@
       <c r="G1" t="s">
         <v>14</v>
       </c>
+      <c r="H1" t="s">
+        <v>41</v>
+      </c>
     </row>
-    <row r="2" spans="1:7" ht="24" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:8" ht="24" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>1</v>
       </c>
@@ -830,8 +842,11 @@
       <c r="G2" t="e" vm="2">
         <v>#VALUE!</v>
       </c>
+      <c r="H2" t="s">
+        <v>42</v>
+      </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>2</v>
       </c>
@@ -849,6 +864,9 @@
       </c>
       <c r="F3">
         <v>2</v>
+      </c>
+      <c r="H3" t="s">
+        <v>43</v>
       </c>
     </row>
   </sheetData>
@@ -860,7 +878,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0E2F9387-600B-D541-9BC6-6CD6305CE841}">
   <dimension ref="A1:H3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView topLeftCell="B1" workbookViewId="0">
       <selection activeCell="C33" sqref="C33"/>
     </sheetView>
   </sheetViews>

</xml_diff>